<commit_message>
fin forward bulkhead assembly, lower body masses
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/RORO/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="16840" yWindow="460" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mass budget" sheetId="1" r:id="rId1"/>
     <sheet name="Component weights" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <t>Component</t>
   </si>
@@ -72,30 +72,15 @@
     <t>measured, scaled</t>
   </si>
   <si>
-    <t>Phenolic tube, 115cm</t>
-  </si>
-  <si>
     <t>estimated</t>
   </si>
   <si>
-    <t>tube carbon fiber reinforcement</t>
-  </si>
-  <si>
-    <t>Recover/payload bulkhead</t>
-  </si>
-  <si>
-    <t>estimated, based on measured fiberglass reinforced 10cm tube</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
     <t>Recovery</t>
   </si>
   <si>
-    <t>Nosecone release</t>
-  </si>
-  <si>
     <t>Recovery batteries 4x 2s 300mAh</t>
   </si>
   <si>
@@ -129,54 +114,27 @@
     <t>upper bulkhead</t>
   </si>
   <si>
-    <t>Phenolic tube, 90cm</t>
-  </si>
-  <si>
     <t>Trim Weight</t>
   </si>
   <si>
     <t>Requirement</t>
   </si>
   <si>
-    <t>coupler tube</t>
-  </si>
-  <si>
     <t>motor tube 70cm</t>
   </si>
   <si>
-    <t>centering rings 5x, 3mm plywood</t>
-  </si>
-  <si>
     <t>thrust plate 3mm aluminium</t>
   </si>
   <si>
-    <t>fins carbon fiber skin</t>
-  </si>
-  <si>
     <t>fins carbon fiber reinforced attachement</t>
   </si>
   <si>
     <t>aeropack retainer with screws</t>
   </si>
   <si>
-    <t>estimated based on density</t>
-  </si>
-  <si>
-    <t>fins, plywood core (20cm x 30cm, 4mm)  3x</t>
-  </si>
-  <si>
-    <t>estimated based on density, 670kg/m3</t>
-  </si>
-  <si>
-    <t>estimated based on density, 2.7g/cm3</t>
-  </si>
-  <si>
     <t>Total (without motor)</t>
   </si>
   <si>
-    <t>forum</t>
-  </si>
-  <si>
     <t>weight (kg)</t>
   </si>
   <si>
@@ -289,6 +247,39 @@
   </si>
   <si>
     <t>rest</t>
+  </si>
+  <si>
+    <t>centering rings 5x, 4mm plywood</t>
+  </si>
+  <si>
+    <t>coupler tube with carbon reinforcement</t>
+  </si>
+  <si>
+    <t>Phenolic tube, 90cm with carbon reinforcement</t>
+  </si>
+  <si>
+    <t>Phenolic tube, 115cm with carbon reinforcement</t>
+  </si>
+  <si>
+    <t>forum, scaled</t>
+  </si>
+  <si>
+    <t>Recovery structure/bulkhead</t>
+  </si>
+  <si>
+    <t>Recovery/payload bulkhead</t>
+  </si>
+  <si>
+    <t>Nosecone release bars</t>
+  </si>
+  <si>
+    <t>fins, 9mm plywood with balsa core, + cfrp reinforcemnt</t>
+  </si>
+  <si>
+    <t>124, 125, 122g</t>
+  </si>
+  <si>
+    <t>fin forward bulkhead 12mm plywood (with nuts)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +287,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -373,11 +364,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -657,15 +648,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D58"/>
+  <dimension ref="A2:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -676,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -745,7 +736,7 @@
       </c>
       <c r="B12" s="9">
         <f>B13+B17+B24+B25</f>
-        <v>9.7759836065573769</v>
+        <v>9.5630000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,89 +745,87 @@
       </c>
       <c r="B13" s="6">
         <f>SUM(B14:B16)</f>
-        <v>2.5059836065573773</v>
+        <v>2.1430000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B14" s="5">
-        <f>1.022*115/122</f>
-        <v>0.96336065573770491</v>
+        <v>1.5629999999999999</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5">
-        <f>1*115/122</f>
-        <v>0.94262295081967218</v>
+        <v>79</v>
+      </c>
+      <c r="B15">
+        <v>0.48</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="B16">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <f>SUM(B18:B23)</f>
-        <v>1.27</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="B18">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>0.02</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>0.1</v>
@@ -847,18 +836,18 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>0.2</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0.7</v>
@@ -869,18 +858,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -888,7 +877,7 @@
     </row>
     <row r="27" spans="1:3" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" s="9"/>
     </row>
@@ -897,262 +886,252 @@
         <v>2</v>
       </c>
       <c r="B28" s="6">
-        <f>SUM(B29:B39)</f>
-        <v>3.8730054644808747</v>
+        <f>SUM(B29:B38)</f>
+        <v>3.3233661202185796</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B29" s="5">
-        <f>1.022*90/122</f>
-        <v>0.75393442622950824</v>
+        <v>1.1539999999999999</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="5">
-        <f>1*90/122</f>
-        <v>0.73770491803278693</v>
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>0.441</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B31">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32">
-        <v>0.3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="5">
+      <c r="A32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5">
         <f>0.407*70/91.5</f>
         <v>0.31136612021857923</v>
       </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="C33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="B34">
-        <f>5*0.02</f>
-        <v>0.1</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B35">
         <v>0.08</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B36">
-        <f>3*0.16</f>
-        <v>0.48</v>
+        <f>0.125+0.124+0.122</f>
+        <v>0.371</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B37">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B38">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39">
-        <v>0.11</v>
-      </c>
-      <c r="C39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="9">
         <f>B4+B12+B28</f>
-        <v>15.642989071038251</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="1">
+        <v>14.88036612021858</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="1">
         <v>2.9889999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47">
+        <v>1.1950000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B48">
-        <v>1.1950000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49">
-        <f>B47-B48</f>
+        <f>B46-B47</f>
         <v>1.7939999999999998</v>
       </c>
-      <c r="C49">
+      <c r="C48">
         <v>1.1399999999999999</v>
       </c>
-      <c r="D49">
-        <f>B49-C49</f>
+      <c r="D48">
+        <f>B48-C48</f>
         <v>0.65399999999999991</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4.8840000000000003</v>
+      </c>
+    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4.8840000000000003</v>
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51">
+        <v>2.508</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B52">
-        <v>2.508</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53">
-        <f>B51-B52</f>
+        <f>B50-B51</f>
         <v>2.3760000000000003</v>
       </c>
-      <c r="C53">
+      <c r="C52">
         <v>1.53</v>
       </c>
-      <c r="D53">
-        <f>B53-C53</f>
+      <c r="D52">
+        <f>B52-C52</f>
         <v>0.84600000000000031</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="1">
+        <v>6.9119999999999999</v>
+      </c>
+    </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="1">
-        <v>6.9119999999999999</v>
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55">
+        <v>3.948</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B56">
-        <v>3.948</v>
+        <f>B54-B55</f>
+        <v>2.964</v>
+      </c>
+      <c r="C56">
+        <v>1.9259999999999999</v>
+      </c>
+      <c r="D56">
+        <f>B56-C56</f>
+        <v>1.038</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57">
-        <f>B55-B56</f>
-        <v>2.964</v>
-      </c>
-      <c r="C57">
-        <v>1.9259999999999999</v>
-      </c>
-      <c r="D57">
-        <f>B57-C57</f>
-        <v>1.038</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
-        <v>85</v>
-      </c>
-      <c r="D58" t="s">
-        <v>86</v>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C46" r:id="rId1"/>
+    <hyperlink ref="C45" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1161,12 +1140,12 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1175,13 +1154,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1191,7 +1170,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.40699999999999997</v>
@@ -1200,12 +1179,12 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>0.8</v>
@@ -1214,12 +1193,12 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1.022</v>
@@ -1228,12 +1207,12 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>0.59399999999999997</v>
@@ -1244,7 +1223,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>0.23200000000000001</v>
@@ -1255,7 +1234,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>0.30099999999999999</v>
@@ -1264,12 +1243,12 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>7.1999999999999995E-2</v>
@@ -1278,12 +1257,12 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0.29499999999999998</v>
@@ -1294,7 +1273,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>0.13</v>
@@ -1303,28 +1282,28 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0.09</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>0.72099999999999997</v>
@@ -1333,39 +1312,39 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>6.6E-3</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>3.7999999999999999E-2</v>
@@ -1376,7 +1355,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B22">
         <v>6.2E-2</v>
@@ -1387,7 +1366,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B23">
         <v>5.8999999999999997E-2</v>

</xml_diff>

<commit_message>
mass budget for the glider
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/RORO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/RocketCompetition/Git/RORO/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="460" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="24820" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mass budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Component weights" sheetId="2" r:id="rId2"/>
+    <sheet name="Payload Budget" sheetId="3" r:id="rId2"/>
+    <sheet name="Component weights" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
   <si>
     <t>Component</t>
   </si>
@@ -280,6 +281,66 @@
   </si>
   <si>
     <t>fin forward bulkhead 12mm plywood (with nuts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component </t>
+  </si>
+  <si>
+    <t>Mass (g)</t>
+  </si>
+  <si>
+    <t>Cost (EUR)</t>
+  </si>
+  <si>
+    <t>Autopilot</t>
+  </si>
+  <si>
+    <t>Pitot tube</t>
+  </si>
+  <si>
+    <t>Servomotors x 3</t>
+  </si>
+  <si>
+    <t>UBLOX</t>
+  </si>
+  <si>
+    <t>https://drotek.com/shop/en/drotek-parts/792-xl-rtk-gps-neo-m8p-rover.html</t>
+  </si>
+  <si>
+    <t>Xbee</t>
+  </si>
+  <si>
+    <t>http://www.mouser.ch/ProductDetail/Digi-International/XB8-DMUS-002/?qs=%2fha2pyFaduhamZ1j%2fTvqvLufopfOt%252bEr7wrfpr46JtwlpBsVij4AWA%3d%3d</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Cabling</t>
+  </si>
+  <si>
+    <t>Mounting</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>Hinges + locking mech</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Total without margin</t>
+  </si>
+  <si>
+    <t>Total with 20% margin</t>
+  </si>
+  <si>
+    <t>Ground Station GPS RTK</t>
   </si>
 </sst>
 </file>
@@ -289,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -336,13 +397,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -358,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -370,6 +467,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -650,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+    <sheetView zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -1136,6 +1247,241 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="14">
+        <v>10.54</v>
+      </c>
+      <c r="C3" s="14">
+        <v>100</v>
+      </c>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="14">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14">
+        <v>20</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="16">
+        <f>4.5*3</f>
+        <v>13.5</v>
+      </c>
+      <c r="C5" s="14">
+        <v>90</v>
+      </c>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="17">
+        <v>23</v>
+      </c>
+      <c r="C6" s="17">
+        <v>350</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>50</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="14">
+        <v>36</v>
+      </c>
+      <c r="C8" s="14">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="14">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14">
+        <v>3</v>
+      </c>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="14">
+        <v>100</v>
+      </c>
+      <c r="C12" s="14">
+        <v>30</v>
+      </c>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="14">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="14">
+        <v>20</v>
+      </c>
+      <c r="C14" s="14">
+        <v>30</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="22">
+        <f t="shared" ref="B15:C15" si="0">SUM(B3:B14)</f>
+        <v>236.04</v>
+      </c>
+      <c r="C15" s="16">
+        <f t="shared" si="0"/>
+        <v>694</v>
+      </c>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="22">
+        <f t="shared" ref="B16:C16" si="1">B15+20/100*B15</f>
+        <v>283.24799999999999</v>
+      </c>
+      <c r="C16" s="16">
+        <f t="shared" si="1"/>
+        <v>832.8</v>
+      </c>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="14">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>

</xml_diff>

<commit_message>
mass budget update with measured weights
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/RocketCompetition/Git/RORO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="24820" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16840" yWindow="460" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Mass budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Payload Budget" sheetId="3" r:id="rId2"/>
-    <sheet name="Component weights" sheetId="2" r:id="rId3"/>
+    <sheet name="Measured Mass budget RORO1" sheetId="4" r:id="rId1"/>
+    <sheet name="Design Mass budget RORO1" sheetId="1" r:id="rId2"/>
+    <sheet name="Payload Budget" sheetId="3" r:id="rId3"/>
+    <sheet name="Component weights" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
   <si>
     <t>Component</t>
   </si>
@@ -341,14 +342,117 @@
   </si>
   <si>
     <t>Ground Station GPS RTK</t>
+  </si>
+  <si>
+    <t>m8 threaded rod: 87.3g / 283mm</t>
+  </si>
+  <si>
+    <t>g/mm</t>
+  </si>
+  <si>
+    <t>plywood birch (thick)</t>
+  </si>
+  <si>
+    <t>g/mm3</t>
+  </si>
+  <si>
+    <t>weitght [kg]</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>weight with margin [kg]</t>
+  </si>
+  <si>
+    <t>Nosecone with deployment</t>
+  </si>
+  <si>
+    <t>(initial estimate 4.2kg)</t>
+  </si>
+  <si>
+    <t>Upper body</t>
+  </si>
+  <si>
+    <t>Upper body with threaded rods</t>
+  </si>
+  <si>
+    <t>parachute</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>Recovery bay with batteries &amp; co2</t>
+  </si>
+  <si>
+    <t>Recovery bulkhead screws and parachute eyebolts</t>
+  </si>
+  <si>
+    <t>lower body</t>
+  </si>
+  <si>
+    <t>Lower Body with retainer, threaded rods</t>
+  </si>
+  <si>
+    <t>gopro bulkhead</t>
+  </si>
+  <si>
+    <t>gopro</t>
+  </si>
+  <si>
+    <t>gopro bulkhead screws</t>
+  </si>
+  <si>
+    <t>eybolts for recovery</t>
+  </si>
+  <si>
+    <t>avionics (lower body)</t>
+  </si>
+  <si>
+    <t>railguides</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>total with margin</t>
+  </si>
+  <si>
+    <t>system margin</t>
+  </si>
+  <si>
+    <t>total with system margin</t>
+  </si>
+  <si>
+    <t>estimated trim weight</t>
+  </si>
+  <si>
+    <t>M2400T</t>
+  </si>
+  <si>
+    <t>ideal weight</t>
+  </si>
+  <si>
+    <t>trim weight</t>
+  </si>
+  <si>
+    <t>trim weight plus margin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -455,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -481,6 +585,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -759,10 +866,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>3.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2">
+        <f>E2*C2</f>
+        <v>3.8500000000000005</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3">
+        <v>2.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>E3*C3</f>
+        <v>2.4</v>
+      </c>
+      <c r="H3">
+        <f>SUM(C3:C7)</f>
+        <v>9.1859999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4">
+        <v>1.6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>E4*C4</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F5">
+        <f>E5*C5</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F15" si="0">E6*C6</f>
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <f>0.04+0.152</f>
+        <v>0.192</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8">
+        <v>4.0350000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4.0350000000000001</v>
+      </c>
+      <c r="H8">
+        <f>SUM(C8:C14)</f>
+        <v>4.6849999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>0.04</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12">
+        <v>0.152</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13">
+        <v>0.127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14">
+        <f>2*0.02</f>
+        <v>0.04</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1.5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="1">
+        <f>SUM(C2:C16)</f>
+        <v>17.870999999999999</v>
+      </c>
+      <c r="F17" s="23">
+        <f>SUM(F2:F16)</f>
+        <v>18.870999999999999</v>
+      </c>
+      <c r="G17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="F18" s="24">
+        <v>1.05</v>
+      </c>
+      <c r="G18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="F19" s="25">
+        <f>F17*F18</f>
+        <v>19.814550000000001</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="F20" s="23">
+        <f>F19-C17</f>
+        <v>1.9435500000000019</v>
+      </c>
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="E22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22">
+        <v>20.55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="F23" s="24">
+        <f>F22-F19</f>
+        <v>0.73545000000000016</v>
+      </c>
+      <c r="G23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="F24" s="24">
+        <f>F22-C17</f>
+        <v>2.679000000000002</v>
+      </c>
+      <c r="G24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="F25" s="24">
+        <f>F24-F23</f>
+        <v>1.9435500000000019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D57"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A27" zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1246,11 +1776,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1431,11 +1961,11 @@
         <v>101</v>
       </c>
       <c r="B15" s="22">
-        <f t="shared" ref="B15:C15" si="0">SUM(B3:B14)</f>
+        <f>SUM(B3:B14)</f>
         <v>236.04</v>
       </c>
       <c r="C15" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(C3:C14)</f>
         <v>694</v>
       </c>
       <c r="D15" s="12"/>
@@ -1445,11 +1975,11 @@
         <v>102</v>
       </c>
       <c r="B16" s="22">
-        <f t="shared" ref="B16:C16" si="1">B15+20/100*B15</f>
+        <f>B15+20/100*B15</f>
         <v>283.24799999999999</v>
       </c>
       <c r="C16" s="16">
-        <f t="shared" si="1"/>
+        <f>C15+20/100*C15</f>
         <v>832.8</v>
       </c>
       <c r="D16" s="12"/>
@@ -1481,12 +2011,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1721,7 +2251,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26">
+        <f>87.3/283</f>
+        <v>0.30848056537102475</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27">
+        <f>708/((200*400-79*49)*14.2)</f>
+        <v>6.5492985497743916E-4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
roro1 fix motor & propellant mass, add trim mass for inertia moments
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/working/IREC/RORO/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Measured Mass budget RORO1" sheetId="4" r:id="rId1"/>
-    <sheet name="Design Mass budget RORO1" sheetId="1" r:id="rId2"/>
+    <sheet name="Initial Mass budget RORO1" sheetId="1" r:id="rId2"/>
     <sheet name="Payload Budget" sheetId="3" r:id="rId3"/>
     <sheet name="Component weights" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="145">
   <si>
     <t>Component</t>
   </si>
@@ -444,6 +444,27 @@
   </si>
   <si>
     <t>trim weight plus margin</t>
+  </si>
+  <si>
+    <t>Motor weight</t>
+  </si>
+  <si>
+    <t>RockSim</t>
+  </si>
+  <si>
+    <t>Thurstcurve.org</t>
+  </si>
+  <si>
+    <t>propellant weight</t>
+  </si>
+  <si>
+    <t>case (difference)</t>
+  </si>
+  <si>
+    <t>Lift off weight</t>
+  </si>
+  <si>
+    <t>After burnout</t>
   </si>
 </sst>
 </file>
@@ -559,7 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -588,6 +609,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -866,13 +888,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
@@ -1173,7 +1199,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>129</v>
@@ -1190,7 +1216,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="F18" s="24">
         <v>1.05</v>
@@ -1199,7 +1225,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="F19" s="25">
         <f>F17*F18</f>
@@ -1209,7 +1235,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="F20" s="23">
         <f>F19-C17</f>
@@ -1219,10 +1245,16 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>139</v>
+      </c>
+      <c r="K21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="E22" t="s">
         <v>134</v>
@@ -1233,8 +1265,18 @@
       <c r="G22" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22">
+        <f>27.033-20.55</f>
+        <v>6.4830000000000005</v>
+      </c>
+      <c r="K22">
+        <v>6.4509999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="F23" s="24">
         <f>F22-F19</f>
@@ -1243,8 +1285,18 @@
       <c r="G23" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23">
+        <f>27.033-23.34</f>
+        <v>3.6930000000000014</v>
+      </c>
+      <c r="K23">
+        <v>3.6930000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="F24" s="24">
         <f>F22-C17</f>
@@ -1253,33 +1305,54 @@
       <c r="G24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>142</v>
+      </c>
+      <c r="J24">
+        <f>J22-J23</f>
+        <v>2.7899999999999991</v>
+      </c>
+      <c r="K24">
+        <f>K22-K23</f>
+        <v>2.7579999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="F25" s="24">
-        <f>F24-F23</f>
-        <v>1.9435500000000019</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F25" s="26">
+        <f>F22+J22</f>
+        <v>27.033000000000001</v>
+      </c>
+      <c r="G25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="24">
+        <f>F25-J23</f>
+        <v>23.34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
   </sheetData>
@@ -1292,7 +1365,7 @@
   <dimension ref="A2:D57"/>
   <sheetViews>
     <sheetView topLeftCell="A27" zoomScale="113" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
definitive mass budget for report
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
   <si>
     <t>Component</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Nosecone with deployment</t>
   </si>
   <si>
-    <t>(initial estimate 4.2kg)</t>
-  </si>
-  <si>
     <t>Upper body</t>
   </si>
   <si>
@@ -380,9 +377,6 @@
     <t>parachute</t>
   </si>
   <si>
-    <t>payload</t>
-  </si>
-  <si>
     <t>requirement</t>
   </si>
   <si>
@@ -465,6 +459,21 @@
   </si>
   <si>
     <t>After burnout</t>
+  </si>
+  <si>
+    <t>payload glider</t>
+  </si>
+  <si>
+    <t>payload weight</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>to get to 4kg total</t>
+  </si>
+  <si>
+    <t>Total weight without payload &amp; motor</t>
   </si>
 </sst>
 </file>
@@ -888,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,28 +929,25 @@
         <v>111</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="E2">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="F2">
         <f>E2*C2</f>
-        <v>3.8500000000000005</v>
-      </c>
-      <c r="G2" t="s">
-        <v>112</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
       </c>
       <c r="C3">
         <v>2.4</v>
@@ -957,14 +963,14 @@
         <v>2.4</v>
       </c>
       <c r="H3">
-        <f>SUM(C3:C7)</f>
+        <f>SUM(C3:C8)</f>
         <v>9.1859999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4">
         <v>1.6</v>
@@ -983,112 +989,115 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <f>4-C6</f>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E5">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="F5">
         <f>E5*C5</f>
-        <v>4.4000000000000004</v>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="G5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C6">
-        <v>0.99399999999999999</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>145</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F15" si="0">E6*C6</f>
-        <v>0.99399999999999999</v>
+        <f>E6*C6</f>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C7">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F16" si="0">E7*C7</f>
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8">
         <f>0.04+0.152</f>
         <v>0.192</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>0.192</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
         <v>4.0350000000000001</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>4.0350000000000001</v>
       </c>
-      <c r="H8">
-        <f>SUM(C8:C14)</f>
+      <c r="H9">
+        <f>SUM(C9:C15)</f>
         <v>4.6849999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10">
-        <v>8.6999999999999994E-2</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1098,16 +1107,16 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C11">
-        <v>0.04</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1117,16 +1126,16 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12">
-        <v>0.152</v>
+        <v>0.04</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1136,16 +1145,16 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0.152</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C13">
-        <v>0.127</v>
+        <v>0.152</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1155,190 +1164,206 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.127</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C14">
+        <v>0.127</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15">
         <f>2*0.02</f>
         <v>0.04</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16">
         <v>0.5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>1.5</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="1">
-        <f>SUM(C2:C16)</f>
-        <v>17.870999999999999</v>
-      </c>
-      <c r="F17" s="23">
-        <f>SUM(F2:F16)</f>
-        <v>18.870999999999999</v>
-      </c>
-      <c r="G17" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="F18" s="24">
-        <v>1.05</v>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUM(C2:C17)</f>
+        <v>17.370999999999999</v>
+      </c>
+      <c r="F18" s="23">
+        <f>SUM(F2:F17)</f>
+        <v>18.570999999999998</v>
       </c>
       <c r="G18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="F19" s="25">
-        <f>F17*F18</f>
-        <v>19.814550000000001</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>132</v>
+      <c r="F19" s="24">
+        <v>1.05</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="F20" s="23">
-        <f>F19-C17</f>
-        <v>1.9435500000000019</v>
-      </c>
-      <c r="G20" t="s">
-        <v>133</v>
+      <c r="F20" s="25">
+        <f>F18*F19</f>
+        <v>19.499549999999999</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="J21" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" t="s">
-        <v>140</v>
+      <c r="F21" s="23">
+        <f>F20-C18</f>
+        <v>2.1285500000000006</v>
+      </c>
+      <c r="G21" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="E22" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22">
-        <v>20.55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>135</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>137</v>
+      </c>
+      <c r="K22" t="s">
         <v>138</v>
       </c>
-      <c r="J22">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="E23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+      <c r="I23" t="s">
+        <v>136</v>
+      </c>
+      <c r="J23">
         <f>27.033-20.55</f>
         <v>6.4830000000000005</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>6.4509999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="F23" s="24">
-        <f>F22-F19</f>
-        <v>0.73545000000000016</v>
-      </c>
-      <c r="G23" t="s">
-        <v>136</v>
-      </c>
-      <c r="I23" t="s">
-        <v>141</v>
-      </c>
-      <c r="J23">
-        <f>27.033-23.34</f>
-        <v>3.6930000000000014</v>
-      </c>
-      <c r="K23">
-        <v>3.6930000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="F24" s="24">
-        <f>F22-C17</f>
-        <v>2.679000000000002</v>
+        <f>F23-F20</f>
+        <v>0.50045000000000073</v>
       </c>
       <c r="G24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J24">
-        <f>J22-J23</f>
-        <v>2.7899999999999991</v>
+        <f>27.033-23.34</f>
+        <v>3.6930000000000014</v>
       </c>
       <c r="K24">
-        <f>K22-K23</f>
-        <v>2.7579999999999996</v>
+        <v>3.6930000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="F25" s="26">
-        <f>F22+J22</f>
-        <v>27.033000000000001</v>
+      <c r="F25" s="24">
+        <f>F23-C18</f>
+        <v>2.6290000000000013</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>135</v>
+      </c>
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25">
+        <f>J23-J24</f>
+        <v>2.7899999999999991</v>
+      </c>
+      <c r="K25">
+        <f>K23-K24</f>
+        <v>2.7579999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="F26" s="24">
-        <f>F25-J23</f>
-        <v>23.34</v>
+      <c r="F26" s="26">
+        <f>F23+J23</f>
+        <v>26.483000000000001</v>
       </c>
       <c r="G26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
+      <c r="F27" s="24">
+        <f>F26-J24</f>
+        <v>22.79</v>
+      </c>
+      <c r="G27" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1354,6 +1379,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32">
+        <f>F23-C5-C6</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
competition flight analysis & update final masses
</commit_message>
<xml_diff>
--- a/mass-budget.xlsx
+++ b/mass-budget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="460" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="16760" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Measured Mass budget RORO1" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="159">
   <si>
     <t>Component</t>
   </si>
@@ -365,9 +365,6 @@
     <t>weight with margin [kg]</t>
   </si>
   <si>
-    <t>Nosecone with deployment</t>
-  </si>
-  <si>
     <t>Upper body</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
     <t>parachute</t>
   </si>
   <si>
-    <t>requirement</t>
-  </si>
-  <si>
     <t>Recovery bay with batteries &amp; co2</t>
   </si>
   <si>
@@ -392,21 +386,12 @@
     <t>Lower Body with retainer, threaded rods</t>
   </si>
   <si>
-    <t>gopro bulkhead</t>
-  </si>
-  <si>
-    <t>gopro</t>
-  </si>
-  <si>
     <t>gopro bulkhead screws</t>
   </si>
   <si>
     <t>eybolts for recovery</t>
   </si>
   <si>
-    <t>avionics (lower body)</t>
-  </si>
-  <si>
     <t>railguides</t>
   </si>
   <si>
@@ -464,25 +449,74 @@
     <t>payload glider</t>
   </si>
   <si>
-    <t>payload weight</t>
-  </si>
-  <si>
-    <t>design</t>
-  </si>
-  <si>
-    <t>to get to 4kg total</t>
-  </si>
-  <si>
     <t>Total weight without payload &amp; motor</t>
+  </si>
+  <si>
+    <t>gopro bulkhead with gopro and backup battery</t>
+  </si>
+  <si>
+    <t>nosecone</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>cable with connector</t>
+  </si>
+  <si>
+    <t>rail</t>
+  </si>
+  <si>
+    <t>slider</t>
+  </si>
+  <si>
+    <t>payload box</t>
+  </si>
+  <si>
+    <t>central M8 bolt with nuts</t>
+  </si>
+  <si>
+    <t>payload nuts</t>
+  </si>
+  <si>
+    <t>small camera</t>
+  </si>
+  <si>
+    <t>payload tungsten block</t>
+  </si>
+  <si>
+    <t>payload battery &amp; imu</t>
+  </si>
+  <si>
+    <t>1U payload total</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>nose</t>
+  </si>
+  <si>
+    <t>M2100G</t>
+  </si>
+  <si>
+    <t>Propellant weight</t>
+  </si>
+  <si>
+    <t>burnout weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -589,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -619,6 +653,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -897,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +944,7 @@
     <col min="9" max="9" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" t="s">
         <v>108</v>
@@ -921,36 +956,40 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>E2*C2</f>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H2">
+        <f>SUM(C2:C7)</f>
+        <v>3.3409999999999997</v>
+      </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="C3">
-        <v>2.4</v>
+        <v>1.611</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -959,21 +998,16 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <f>E3*C3</f>
-        <v>2.4</v>
-      </c>
-      <c r="H3">
-        <f>SUM(C3:C8)</f>
-        <v>9.1859999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+        <f t="shared" ref="F3:F7" si="0">E3*C3</f>
+        <v>1.611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C4">
-        <v>1.6</v>
+        <v>0.15</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -982,58 +1016,52 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <f>E4*C4</f>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>144</v>
       </c>
       <c r="C5">
-        <f>4-C6</f>
-        <v>3</v>
+        <v>0.442</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <f>E5*C5</f>
-        <v>3.1500000000000004</v>
-      </c>
-      <c r="G5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C6">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6">
-        <v>1.2</v>
-      </c>
       <c r="F6">
-        <f>E6*C6</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+        <f t="shared" si="0"/>
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C7">
-        <v>0.99399999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1042,120 +1070,129 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F16" si="0">E7*C7</f>
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8">
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>E8*C8</f>
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="H8">
+        <f>SUM(C8:C13)</f>
+        <v>6.2579999999999991</v>
+      </c>
+      <c r="I8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9">
+        <v>1.6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>E9*C9</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>E10*C10</f>
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="H10">
+        <f>SUM(C10:C11)</f>
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="I10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>E11*C11</f>
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F23" si="1">E12*C12</f>
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13">
         <f>0.04+0.152</f>
         <v>0.192</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9">
-        <v>4.0350000000000001</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>4.0350000000000001</v>
-      </c>
-      <c r="H9">
-        <f>SUM(C9:C15)</f>
-        <v>4.6849999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.20399999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>8.6999999999999994E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12">
-        <v>0.04</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13">
-        <v>0.152</v>
-      </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
@@ -1163,17 +1200,19 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0.152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+        <f t="shared" si="1"/>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C14">
-        <v>0.127</v>
+        <v>4.2919999999999998</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1182,18 +1221,24 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0.127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="H14">
+        <f>SUM(C14:C23)</f>
+        <v>8.3160000000000007</v>
+      </c>
+      <c r="I14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C15">
-        <f>2*0.02</f>
-        <v>0.04</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1202,193 +1247,379 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16">
-        <v>0.5</v>
-      </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
+        <f>E16*C16</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17">
+        <v>0.152</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>E17*C17</f>
+        <v>0.152</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="1">
-        <f>SUM(C2:C17)</f>
-        <v>17.370999999999999</v>
-      </c>
-      <c r="F18" s="23">
-        <f>SUM(F2:F17)</f>
-        <v>18.570999999999998</v>
-      </c>
-      <c r="G18" t="s">
-        <v>128</v>
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <f>4.089-1</f>
+        <v>3.0890000000000004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f>E18*C18</f>
+        <v>3.0890000000000004</v>
+      </c>
+      <c r="H18">
+        <f>SUM(C18:C21)</f>
+        <v>3.3330000000000006</v>
+      </c>
+      <c r="I18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="F19" s="24">
-        <v>1.05</v>
-      </c>
-      <c r="G19" t="s">
-        <v>129</v>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19">
+        <f>0.417-0.2</f>
+        <v>0.21699999999999997</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19:F22" si="2">E19*C19</f>
+        <v>0.21699999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="F20" s="25">
-        <f>F18*F19</f>
-        <v>19.499549999999999</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>130</v>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="F21" s="23">
-        <f>F20-C18</f>
-        <v>2.1285500000000006</v>
-      </c>
-      <c r="G21" t="s">
-        <v>131</v>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="J22" t="s">
-        <v>137</v>
-      </c>
-      <c r="K22" t="s">
-        <v>138</v>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <f>2*0.02</f>
+        <v>0.04</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="E23" t="s">
+      <c r="A23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>0.105</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(C2:C24)</f>
+        <v>17.914999999999996</v>
+      </c>
+      <c r="F25" s="23">
+        <f>SUM(F2:F24)</f>
+        <v>17.914999999999996</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="F26" s="24">
+        <v>1.05</v>
+      </c>
+      <c r="G26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="F27" s="25">
+        <f>F25*F26</f>
+        <v>18.810749999999995</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="F28" s="23">
+        <f>F27-C25</f>
+        <v>0.8957499999999996</v>
+      </c>
+      <c r="G28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="J29" t="s">
         <v>132</v>
       </c>
-      <c r="F23">
+      <c r="K29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="E30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30">
         <v>20</v>
       </c>
-      <c r="G23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I23" t="s">
-        <v>136</v>
-      </c>
-      <c r="J23">
+      <c r="G30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" t="s">
+        <v>131</v>
+      </c>
+      <c r="J30">
         <f>27.033-20.55</f>
         <v>6.4830000000000005</v>
       </c>
-      <c r="K23">
+      <c r="K30">
         <v>6.4509999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="F24" s="24">
-        <f>F23-F20</f>
-        <v>0.50045000000000073</v>
-      </c>
-      <c r="G24" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="F31" s="24">
+        <f>F30-F27</f>
+        <v>1.1892500000000048</v>
+      </c>
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" t="s">
         <v>134</v>
       </c>
-      <c r="I24" t="s">
-        <v>139</v>
-      </c>
-      <c r="J24">
+      <c r="J31">
         <f>27.033-23.34</f>
         <v>3.6930000000000014</v>
       </c>
-      <c r="K24">
+      <c r="K31">
         <v>3.6930000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="F25" s="24">
-        <f>F23-C18</f>
-        <v>2.6290000000000013</v>
-      </c>
-      <c r="G25" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" t="s">
-        <v>140</v>
-      </c>
-      <c r="J25">
-        <f>J23-J24</f>
-        <v>2.7899999999999991</v>
-      </c>
-      <c r="K25">
-        <f>K23-K24</f>
-        <v>2.7579999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="F26" s="26">
-        <f>F23+J23</f>
-        <v>26.483000000000001</v>
-      </c>
-      <c r="G26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="F27" s="24">
-        <f>F26-J24</f>
-        <v>22.79</v>
-      </c>
-      <c r="G27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32">
-        <f>F23-C5-C6</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F32" s="24">
+        <f>F30-C25</f>
+        <v>2.0850000000000044</v>
+      </c>
+      <c r="G32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32">
+        <f>J30-J31</f>
+        <v>2.7899999999999991</v>
+      </c>
+      <c r="K32">
+        <f>K30-K31</f>
+        <v>2.7579999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
+      <c r="F33" s="26">
+        <f>F30+J30</f>
+        <v>26.483000000000001</v>
+      </c>
+      <c r="G33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="F34" s="24">
+        <f>F33-J31</f>
+        <v>22.79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="J38" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39">
+        <f>F30-C10-C11</f>
+        <v>18.983000000000001</v>
+      </c>
+      <c r="E39" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" t="s">
+        <v>131</v>
+      </c>
+      <c r="J39" s="27">
+        <v>7.03</v>
+      </c>
+      <c r="K39">
+        <v>6.9180000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="I40" t="s">
+        <v>157</v>
+      </c>
+      <c r="J40" s="27">
+        <f>J39-J41</f>
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>3.948</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>158</v>
+      </c>
+      <c r="J41" s="27">
+        <v>4.03</v>
+      </c>
+      <c r="K41" s="5">
+        <f>K39-K40</f>
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J42" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2124,7 +2355,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>